<commit_message>
Bump to 0.3.0.  New groupBy and orderBy attributes for the forEach tag.  TagListeners and TagLoopListeners.  New metadata keys for implicit collections processing.  Fix formula bugs when the formula isn't the first text in the cell.  Deploy to Sonatype OSS's Maven Repository.
</commit_message>
<xml_diff>
--- a/jett-core/templates/ForEachTagTemplate.xlsx
+++ b/jett-core/templates/ForEachTagTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="16875" windowHeight="9975"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="16875" windowHeight="9975" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="VertVert" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <sheet name="limit" sheetId="7" r:id="rId7"/>
     <sheet name="groupRows" sheetId="8" r:id="rId8"/>
     <sheet name="groupCols" sheetId="9" r:id="rId9"/>
+    <sheet name="groupBy" sheetId="10" r:id="rId10"/>
+    <sheet name="orderBy" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="31">
   <si>
     <t>City</t>
   </si>
@@ -97,6 +99,24 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${division.teams}" var="team" copyRight="true" groupDir="cols" collapse="${division.name.equals('Northwest')}"&gt;${team.city}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${teams}" var="division" groupBy="divisionName"&gt;Division: ${division.obj.divisionName}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${division.items}" var="team"&gt;${team.city}</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>${team.pct}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${teams}" var="team" orderBy="divisionName desc;pct"&gt;${team.divisionName}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${teams}" var="division" groupBy="divisionName" orderBy="divisionName desc;pct"&gt;Division: ${division.obj.divisionName}</t>
   </si>
 </sst>
 </file>
@@ -581,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -694,6 +714,172 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ticket 22: Change AttributeEvaluator back to AttributeUtil and pass a TagContext to each AttributeUtil method.  Ticket 25: Support jAgg 0.8.1, which looks for "get("property")" if "getProperty()" isn't found.  Ticket 31: Option to evaluate formulas after transformation; option to set the force formula recalculation flag.  No ticket: Don't crash if a numeric cell is found in a block for implicit collections processing; fix bad implicit collections processing block if either "left" or "right" specified but not both (introduced in JETT 0.3.0).
</commit_message>
<xml_diff>
--- a/jett-core/templates/ForEachTagTemplate.xlsx
+++ b/jett-core/templates/ForEachTagTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="16875" windowHeight="9975" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="16875" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="VertVert" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>&lt;jt:forEach items="${division.teams}" var="team" copyRight="true" groupDir="cols" collapse="${division.name.equals('Northwest')}"&gt;${team.city}</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${teams}" var="division" groupBy="divisionName"&gt;Division: ${division.obj.divisionName}</t>
-  </si>
-  <si>
     <t>&lt;jt:forEach items="${division.items}" var="team"&gt;${team.city}</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${teams}" var="division" groupBy="divisionName" orderBy="divisionName desc;pct"&gt;Division: ${division.obj.divisionName}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${teams}" var="division" groupBy="division_name"&gt;Division: ${division.obj.divisionName}</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -722,7 +722,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -759,7 +759,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -786,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -798,7 +798,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -840,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Ticket 49 - Implicit sheet cloning, controlled by a collection expression in the sheet name, with abbreviated metadata keys. Ticket 50 - Created the varStatus attribute for looping tags, exposing a LoopTagStatus bean containing the index, first, last, and numIterations properties.  Implicit collections processing now has the varStatus metadata key.  The ForTag extends the varStatus attribute, by exposing a RangedLoopTagStatus, adding the start, end, and step properties.
</commit_message>
<xml_diff>
--- a/jett-core/templates/ForEachTagTemplate.xlsx
+++ b/jett-core/templates/ForEachTagTemplate.xlsx
@@ -18,13 +18,14 @@
     <sheet name="groupCols" sheetId="9" r:id="rId9"/>
     <sheet name="groupBy" sheetId="10" r:id="rId10"/>
     <sheet name="orderBy" sheetId="11" r:id="rId11"/>
+    <sheet name="varStatus" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="43">
   <si>
     <t>City</t>
   </si>
@@ -117,6 +118,42 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${teams}" var="division" groupBy="division_name"&gt;Division: ${division.obj.divisionName}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${divisionsList}" var="division" varStatus="st"&gt;Division: ${division.name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index </t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${division.teams}" var="team" varStatus="teamSt"&gt;${team.city}</t>
+  </si>
+  <si>
+    <t>${team.pct}</t>
+  </si>
+  <si>
+    <t>First?</t>
+  </si>
+  <si>
+    <t>Last?</t>
+  </si>
+  <si>
+    <t>${st.first}</t>
+  </si>
+  <si>
+    <t>${st.last}</t>
+  </si>
+  <si>
+    <t>${teamSt.first}</t>
+  </si>
+  <si>
+    <t>${teamSt.last}&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${st.index} of ${st.numIterations}</t>
+  </si>
+  <si>
+    <t>${teamSt.index} of ${teamSt.numIterations}</t>
   </si>
 </sst>
 </file>
@@ -264,12 +301,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -612,13 +650,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -660,13 +698,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -732,13 +770,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -815,13 +853,13 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -880,6 +918,100 @@
     <mergeCell ref="I1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -899,13 +1031,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="F1" t="s">
         <v>9</v>
       </c>
@@ -945,13 +1077,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1151,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1028,7 +1160,7 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1039,14 +1171,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1055,14 +1187,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1071,14 +1203,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1087,14 +1219,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1139,7 +1271,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1151,7 +1283,7 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1165,14 +1297,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1181,14 +1313,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1197,14 +1329,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1213,14 +1345,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1375,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,14 +1385,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1325,13 +1457,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1395,13 +1527,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1465,13 +1597,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1508,13 +1640,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1579,7 +1711,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1588,7 +1720,7 @@
       <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1599,14 +1731,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1615,14 +1747,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1631,14 +1763,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1647,14 +1779,14 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>